<commit_message>
develop ui untuk excel ppm dan backend untuk ppm
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Regi Ridho Biyantomo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\to-ppt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8C7D44-BFA4-4B0F-97E3-FCC4079B1938}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3307BD81-2ACC-45FB-BCB9-65F112B34936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3036E" sheetId="5" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'3036E'!$A$1:$H$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Customer</t>
   </si>
@@ -120,6 +121,9 @@
   </si>
   <si>
     <t>Unit Status</t>
+  </si>
+  <si>
+    <t>Hour Meters</t>
   </si>
 </sst>
 </file>
@@ -522,11 +526,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,6 +631,87 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -639,32 +721,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -678,6 +760,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -687,105 +778,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1640,9 +1640,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1680,9 +1680,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1715,26 +1715,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1767,26 +1750,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1962,839 +1928,826 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A14" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="3" width="0.109375" customWidth="1"/>
-    <col min="4" max="4" width="39.88671875" customWidth="1"/>
-    <col min="5" max="5" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" customWidth="1"/>
+    <col min="3" max="3" width="0.140625" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="16"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="49"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="49"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="49"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="49"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="35"/>
-    </row>
-    <row r="7" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="50" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="75"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="75"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="75"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="75"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="34"/>
+    </row>
+    <row r="7" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="52"/>
-    </row>
-    <row r="8" spans="1:8" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="23"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="9" t="s">
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="78"/>
+    </row>
+    <row r="8" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="10" t="s">
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="82" t="s">
+      <c r="D10" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="10" t="s">
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="83">
+      <c r="D11" s="49">
         <v>45960</v>
       </c>
-      <c r="E11" s="89"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="10" t="s">
+      <c r="E11" s="53"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="79" t="s">
+      <c r="C12" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="82" t="s">
+      <c r="D12" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="89"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="11" t="s">
+      <c r="E12" s="53"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="89"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="11" t="s">
+      <c r="E13" s="53"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="84"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="10" t="s">
+      <c r="D14" s="50"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="79" t="s">
+      <c r="C15" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="82" t="s">
+      <c r="D15" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="89"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="17"/>
-      <c r="B16" s="12" t="s">
+      <c r="E15" s="53"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="80" t="s">
+      <c r="C16" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="85" t="s">
+      <c r="D16" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="89"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="17"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="89"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="89"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="17"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="18"/>
-      <c r="B28" s="36" t="s">
+      <c r="E16" s="53"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
+      <c r="B27" s="84"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="76"/>
-      <c r="D28" s="77" t="s">
+      <c r="C28" s="87"/>
+      <c r="D28" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="17"/>
-      <c r="B29" s="89"/>
-      <c r="C29" s="89"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="62" t="s">
+      <c r="E28" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="16"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="62" t="s">
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="62" t="s">
+      <c r="F30" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="62"/>
-      <c r="H30" s="62"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="62"/>
-      <c r="B31" s="33" t="s">
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="69"/>
+      <c r="B31" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C31" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="63"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="32" t="s">
+      <c r="D31" s="70"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="G31" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="32" t="s">
+      <c r="H31" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="40">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="54">
         <v>1</v>
       </c>
-      <c r="B32" s="56"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="41"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="41"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="41"/>
-      <c r="B35" s="57"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="41"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="2"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="41"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="41"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="41"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="41"/>
-      <c r="B40" s="57"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="27"/>
-    </row>
-    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="42"/>
-      <c r="B41" s="58"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="28"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="40">
+      <c r="B32" s="57"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="55"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="55"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="55"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="55"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="55"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="55"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="55"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="55"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="26"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="56"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="27"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="54">
         <v>2</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="67"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="70"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="41"/>
-      <c r="B43" s="57"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="70"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="41"/>
-      <c r="B44" s="57"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="70"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="41"/>
-      <c r="B45" s="57"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="70"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="41"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="70"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="41"/>
-      <c r="B47" s="57"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="70"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="41"/>
-      <c r="B48" s="57"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="70"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="41"/>
-      <c r="B49" s="57"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="70"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="41"/>
-      <c r="B50" s="57"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="70"/>
-    </row>
-    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="42"/>
-      <c r="B51" s="58"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="28"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="40">
+      <c r="B42" s="57"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="42"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="55"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="42"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="55"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="42"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="55"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="42"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="55"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="42"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="55"/>
+      <c r="B47" s="58"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="42"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="55"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="42"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="55"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="42"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="55"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="42"/>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="56"/>
+      <c r="B51" s="59"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="65"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="27"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="54">
         <v>3</v>
       </c>
-      <c r="B52" s="56"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="67"/>
-      <c r="G52" s="68"/>
-      <c r="H52" s="70"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="41"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="31"/>
-      <c r="H53" s="70"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="41"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="69"/>
-      <c r="H54" s="70"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="41"/>
-      <c r="B55" s="57"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="70"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="41"/>
-      <c r="B56" s="57"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="70"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="41"/>
-      <c r="B57" s="57"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="46"/>
-      <c r="E57" s="38"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="70"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="41"/>
-      <c r="B58" s="57"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="46"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="70"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="41"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="46"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="70"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="41"/>
-      <c r="B60" s="57"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="46"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="29"/>
-      <c r="H60" s="70"/>
-    </row>
-    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="42"/>
-      <c r="B61" s="58"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="28"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="40">
+      <c r="B52" s="57"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="63"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="42"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="55"/>
+      <c r="B53" s="58"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="64"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="42"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="55"/>
+      <c r="B54" s="58"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="64"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="42"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="55"/>
+      <c r="B55" s="58"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="61"/>
+      <c r="E55" s="64"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="42"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="55"/>
+      <c r="B56" s="58"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="61"/>
+      <c r="E56" s="64"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="42"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="55"/>
+      <c r="B57" s="58"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="61"/>
+      <c r="E57" s="64"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="30"/>
+      <c r="H57" s="42"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="55"/>
+      <c r="B58" s="58"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="64"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="42"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="55"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="61"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="42"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="55"/>
+      <c r="B60" s="58"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="61"/>
+      <c r="E60" s="64"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="42"/>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="56"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="62"/>
+      <c r="E61" s="65"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="27"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="54">
         <v>4</v>
       </c>
-      <c r="B62" s="56"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="44"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="67"/>
-      <c r="G62" s="68"/>
-      <c r="H62" s="27"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="41"/>
-      <c r="B63" s="57"/>
-      <c r="C63" s="45"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="38"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="31"/>
-      <c r="H63" s="2"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="41"/>
-      <c r="B64" s="57"/>
-      <c r="C64" s="45"/>
-      <c r="D64" s="46"/>
-      <c r="E64" s="38"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="69"/>
-      <c r="H64" s="27"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A65" s="41"/>
-      <c r="B65" s="57"/>
-      <c r="C65" s="45"/>
-      <c r="D65" s="46"/>
-      <c r="E65" s="38"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="27"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="41"/>
-      <c r="B66" s="57"/>
-      <c r="C66" s="45"/>
-      <c r="D66" s="46"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="27"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="41"/>
-      <c r="B67" s="57"/>
-      <c r="C67" s="45"/>
-      <c r="D67" s="46"/>
-      <c r="E67" s="38"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="31"/>
-      <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="41"/>
-      <c r="B68" s="57"/>
-      <c r="C68" s="45"/>
-      <c r="D68" s="46"/>
-      <c r="E68" s="38"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="41"/>
-      <c r="B69" s="57"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="46"/>
-      <c r="E69" s="38"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="41"/>
-      <c r="B70" s="57"/>
-      <c r="C70" s="45"/>
-      <c r="D70" s="46"/>
-      <c r="E70" s="38"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="29"/>
-      <c r="H70" s="2"/>
-    </row>
-    <row r="71" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="42"/>
-      <c r="B71" s="58"/>
-      <c r="C71" s="47"/>
-      <c r="D71" s="48"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="26"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-    </row>
-    <row r="72" spans="1:8" ht="69.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="59" t="s">
+      <c r="B62" s="57"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="60"/>
+      <c r="E62" s="63"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="40"/>
+      <c r="H62" s="26"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="55"/>
+      <c r="B63" s="58"/>
+      <c r="C63" s="72"/>
+      <c r="D63" s="61"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="55"/>
+      <c r="B64" s="58"/>
+      <c r="C64" s="72"/>
+      <c r="D64" s="61"/>
+      <c r="E64" s="64"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="41"/>
+      <c r="H64" s="26"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="55"/>
+      <c r="B65" s="58"/>
+      <c r="C65" s="72"/>
+      <c r="D65" s="61"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="26"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="55"/>
+      <c r="B66" s="58"/>
+      <c r="C66" s="72"/>
+      <c r="D66" s="61"/>
+      <c r="E66" s="64"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="26"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="55"/>
+      <c r="B67" s="58"/>
+      <c r="C67" s="72"/>
+      <c r="D67" s="61"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="30"/>
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="55"/>
+      <c r="B68" s="58"/>
+      <c r="C68" s="72"/>
+      <c r="D68" s="61"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="55"/>
+      <c r="B69" s="58"/>
+      <c r="C69" s="72"/>
+      <c r="D69" s="61"/>
+      <c r="E69" s="64"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="55"/>
+      <c r="B70" s="58"/>
+      <c r="C70" s="72"/>
+      <c r="D70" s="61"/>
+      <c r="E70" s="64"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="28"/>
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="56"/>
+      <c r="B71" s="59"/>
+      <c r="C71" s="73"/>
+      <c r="D71" s="62"/>
+      <c r="E71" s="65"/>
+      <c r="F71" s="25"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" ht="69.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B72" s="60"/>
-      <c r="C72" s="60"/>
-      <c r="D72" s="60"/>
-      <c r="E72" s="60"/>
-      <c r="F72" s="60"/>
-      <c r="G72" s="60"/>
-      <c r="H72" s="61"/>
-    </row>
-    <row r="73" spans="1:8" ht="146.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="19"/>
-      <c r="B73" s="20"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
-      <c r="G73" s="20"/>
-      <c r="H73" s="21"/>
+      <c r="B72" s="67"/>
+      <c r="C72" s="67"/>
+      <c r="D72" s="67"/>
+      <c r="E72" s="67"/>
+      <c r="F72" s="67"/>
+      <c r="G72" s="67"/>
+      <c r="H72" s="68"/>
+    </row>
+    <row r="73" spans="1:8" ht="146.44999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="18"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A42:A51"/>
-    <mergeCell ref="B42:B51"/>
-    <mergeCell ref="D42:D51"/>
-    <mergeCell ref="E42:E51"/>
-    <mergeCell ref="D52:D61"/>
+  <mergeCells count="28">
+    <mergeCell ref="E2:H5"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="D18:D27"/>
+    <mergeCell ref="B18:B27"/>
+    <mergeCell ref="C18:C28"/>
+    <mergeCell ref="E18:E27"/>
     <mergeCell ref="A72:H72"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="B30:D30"/>
@@ -2809,13 +2762,13 @@
     <mergeCell ref="B62:B71"/>
     <mergeCell ref="C62:D71"/>
     <mergeCell ref="E62:E71"/>
-    <mergeCell ref="E2:H5"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="D18:D27"/>
-    <mergeCell ref="B18:B27"/>
-    <mergeCell ref="C18:C28"/>
     <mergeCell ref="B52:B61"/>
     <mergeCell ref="E52:E61"/>
+    <mergeCell ref="A42:A51"/>
+    <mergeCell ref="B42:B51"/>
+    <mergeCell ref="D42:D51"/>
+    <mergeCell ref="E42:E51"/>
+    <mergeCell ref="D52:D61"/>
     <mergeCell ref="A52:A61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>